<commit_message>
Diseño de ventanas completadas
</commit_message>
<xml_diff>
--- a/Autorizaciones/Autorizacion_{consecutivo}.xlsx
+++ b/Autorizaciones/Autorizacion_{consecutivo}.xlsx
@@ -18,7 +18,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -130,6 +130,10 @@
       <sz val="18"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FF0000"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -338,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -606,6 +610,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1119,7 +1126,11 @@
           <t>Autorización No.:</t>
         </is>
       </c>
-      <c r="H6" s="96" t="inlineStr"/>
+      <c r="H6" s="96" t="inlineStr">
+        <is>
+          <t>TEST-001</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="6.95" customHeight="1">
       <c r="A7" s="62" t="n"/>
@@ -1145,7 +1156,11 @@
       <c r="D9" s="52" t="n"/>
       <c r="E9" s="52" t="n"/>
       <c r="F9" s="52" t="n"/>
-      <c r="H9" s="36" t="inlineStr"/>
+      <c r="H9" s="97" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="16.5" customHeight="1">
       <c r="A10" s="37" t="inlineStr">
@@ -1180,7 +1195,11 @@
           <t xml:space="preserve">Solicitante: </t>
         </is>
       </c>
-      <c r="B12" s="53" t="inlineStr"/>
+      <c r="B12" s="53" t="inlineStr">
+        <is>
+          <t>Mishell Paola Sandoval Ramirez</t>
+        </is>
+      </c>
       <c r="C12" s="94" t="n"/>
       <c r="D12" s="94" t="n"/>
       <c r="E12" s="1" t="n"/>
@@ -1189,7 +1208,11 @@
           <t>Fecha de solicitud:</t>
         </is>
       </c>
-      <c r="G12" s="97" t="inlineStr"/>
+      <c r="G12" s="98" t="inlineStr">
+        <is>
+          <t>2025/04/03</t>
+        </is>
+      </c>
       <c r="H12" s="94" t="n"/>
     </row>
     <row r="13" ht="24.75" customHeight="1">
@@ -1198,16 +1221,24 @@
           <t>Puesto:</t>
         </is>
       </c>
-      <c r="B13" s="63" t="inlineStr"/>
-      <c r="C13" s="98" t="n"/>
-      <c r="D13" s="98" t="n"/>
+      <c r="B13" s="63" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="C13" s="99" t="n"/>
+      <c r="D13" s="99" t="n"/>
       <c r="E13" s="1" t="n"/>
       <c r="F13" s="21" t="inlineStr">
         <is>
           <t>Fecha requerida:</t>
         </is>
       </c>
-      <c r="G13" s="97" t="inlineStr"/>
+      <c r="G13" s="98" t="inlineStr">
+        <is>
+          <t>2025/04/03</t>
+        </is>
+      </c>
       <c r="H13" s="94" t="n"/>
     </row>
     <row r="14" ht="20.1" customHeight="1">
@@ -1216,16 +1247,24 @@
           <t xml:space="preserve">Área: </t>
         </is>
       </c>
-      <c r="B14" s="63" t="inlineStr"/>
-      <c r="C14" s="98" t="n"/>
-      <c r="D14" s="98" t="n"/>
+      <c r="B14" s="63" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="C14" s="99" t="n"/>
+      <c r="D14" s="99" t="n"/>
       <c r="E14" s="64" t="inlineStr">
         <is>
           <t>Proyecto y/o Contrato:</t>
         </is>
       </c>
-      <c r="G14" s="99" t="inlineStr"/>
-      <c r="H14" s="98" t="n"/>
+      <c r="G14" s="100" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="H14" s="99" t="n"/>
     </row>
     <row r="15" ht="19.5" customHeight="1">
       <c r="D15" s="62" t="n"/>
@@ -1253,38 +1292,70 @@
           <t>Descripción</t>
         </is>
       </c>
-      <c r="E16" s="98" t="n"/>
-      <c r="F16" s="100" t="n"/>
+      <c r="E16" s="99" t="n"/>
+      <c r="F16" s="101" t="n"/>
       <c r="G16" s="61" t="inlineStr">
         <is>
           <t>Observaciones</t>
         </is>
       </c>
-      <c r="H16" s="100" t="n"/>
+      <c r="H16" s="101" t="n"/>
     </row>
     <row r="17" ht="24.75" customHeight="1">
       <c r="A17" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B17" s="9" t="n"/>
-      <c r="C17" s="8" t="n"/>
-      <c r="D17" s="101" t="n"/>
-      <c r="E17" s="98" t="n"/>
-      <c r="F17" s="100" t="n"/>
-      <c r="G17" s="101" t="n"/>
-      <c r="H17" s="100" t="n"/>
+      <c r="B17" s="9" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C17" s="8" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="D17" s="14" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="E17" s="99" t="n"/>
+      <c r="F17" s="101" t="n"/>
+      <c r="G17" s="14" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="H17" s="101" t="n"/>
     </row>
     <row r="18" ht="23.25" customHeight="1">
       <c r="A18" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="B18" s="9" t="n"/>
-      <c r="C18" s="8" t="n"/>
-      <c r="D18" s="101" t="n"/>
-      <c r="E18" s="98" t="n"/>
-      <c r="F18" s="100" t="n"/>
-      <c r="G18" s="101" t="n"/>
-      <c r="H18" s="100" t="n"/>
+      <c r="B18" s="9" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C18" s="8" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="D18" s="14" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="E18" s="99" t="n"/>
+      <c r="F18" s="101" t="n"/>
+      <c r="G18" s="14" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="H18" s="101" t="n"/>
     </row>
     <row r="19" ht="25.5" customHeight="1">
       <c r="A19" s="10" t="n">
@@ -1292,11 +1363,11 @@
       </c>
       <c r="B19" s="18" t="n"/>
       <c r="C19" s="18" t="n"/>
-      <c r="D19" s="101" t="n"/>
-      <c r="E19" s="98" t="n"/>
-      <c r="F19" s="100" t="n"/>
-      <c r="G19" s="101" t="n"/>
-      <c r="H19" s="100" t="n"/>
+      <c r="D19" s="102" t="n"/>
+      <c r="E19" s="99" t="n"/>
+      <c r="F19" s="101" t="n"/>
+      <c r="G19" s="102" t="n"/>
+      <c r="H19" s="101" t="n"/>
     </row>
     <row r="20" ht="25.5" customHeight="1">
       <c r="A20" s="10" t="n">
@@ -1304,11 +1375,11 @@
       </c>
       <c r="B20" s="18" t="n"/>
       <c r="C20" s="18" t="n"/>
-      <c r="D20" s="101" t="n"/>
-      <c r="E20" s="98" t="n"/>
-      <c r="F20" s="100" t="n"/>
-      <c r="G20" s="101" t="n"/>
-      <c r="H20" s="100" t="n"/>
+      <c r="D20" s="102" t="n"/>
+      <c r="E20" s="99" t="n"/>
+      <c r="F20" s="101" t="n"/>
+      <c r="G20" s="102" t="n"/>
+      <c r="H20" s="101" t="n"/>
     </row>
     <row r="21" ht="24" customHeight="1">
       <c r="A21" s="10" t="n">
@@ -1316,11 +1387,11 @@
       </c>
       <c r="B21" s="15" t="n"/>
       <c r="C21" s="15" t="n"/>
-      <c r="D21" s="101" t="n"/>
-      <c r="E21" s="98" t="n"/>
-      <c r="F21" s="100" t="n"/>
-      <c r="G21" s="101" t="n"/>
-      <c r="H21" s="100" t="n"/>
+      <c r="D21" s="102" t="n"/>
+      <c r="E21" s="99" t="n"/>
+      <c r="F21" s="101" t="n"/>
+      <c r="G21" s="102" t="n"/>
+      <c r="H21" s="101" t="n"/>
     </row>
     <row r="22" ht="25.5" customHeight="1">
       <c r="A22" s="10" t="n">
@@ -1328,11 +1399,11 @@
       </c>
       <c r="B22" s="15" t="n"/>
       <c r="C22" s="15" t="n"/>
-      <c r="D22" s="101" t="n"/>
-      <c r="E22" s="98" t="n"/>
-      <c r="F22" s="100" t="n"/>
-      <c r="G22" s="101" t="n"/>
-      <c r="H22" s="100" t="n"/>
+      <c r="D22" s="102" t="n"/>
+      <c r="E22" s="99" t="n"/>
+      <c r="F22" s="101" t="n"/>
+      <c r="G22" s="102" t="n"/>
+      <c r="H22" s="101" t="n"/>
     </row>
     <row r="23" ht="23.25" customHeight="1">
       <c r="A23" s="10" t="n">
@@ -1340,11 +1411,11 @@
       </c>
       <c r="B23" s="15" t="n"/>
       <c r="C23" s="15" t="n"/>
-      <c r="D23" s="101" t="n"/>
-      <c r="E23" s="98" t="n"/>
-      <c r="F23" s="100" t="n"/>
-      <c r="G23" s="101" t="n"/>
-      <c r="H23" s="100" t="n"/>
+      <c r="D23" s="102" t="n"/>
+      <c r="E23" s="99" t="n"/>
+      <c r="F23" s="101" t="n"/>
+      <c r="G23" s="102" t="n"/>
+      <c r="H23" s="101" t="n"/>
     </row>
     <row r="24" ht="23.25" customHeight="1">
       <c r="A24" s="10" t="n">
@@ -1352,9 +1423,9 @@
       </c>
       <c r="B24" s="15" t="n"/>
       <c r="C24" s="15" t="n"/>
-      <c r="D24" s="101" t="n"/>
-      <c r="E24" s="98" t="n"/>
-      <c r="F24" s="100" t="n"/>
+      <c r="D24" s="102" t="n"/>
+      <c r="E24" s="99" t="n"/>
+      <c r="F24" s="101" t="n"/>
       <c r="G24" s="54" t="n"/>
       <c r="H24" s="56" t="n"/>
     </row>
@@ -1364,9 +1435,9 @@
       </c>
       <c r="B25" s="15" t="n"/>
       <c r="C25" s="15" t="n"/>
-      <c r="D25" s="101" t="n"/>
-      <c r="E25" s="98" t="n"/>
-      <c r="F25" s="100" t="n"/>
+      <c r="D25" s="102" t="n"/>
+      <c r="E25" s="99" t="n"/>
+      <c r="F25" s="101" t="n"/>
       <c r="G25" s="54" t="n"/>
       <c r="H25" s="56" t="n"/>
     </row>
@@ -1376,11 +1447,11 @@
       </c>
       <c r="B26" s="15" t="n"/>
       <c r="C26" s="15" t="n"/>
-      <c r="D26" s="101" t="n"/>
-      <c r="E26" s="98" t="n"/>
-      <c r="F26" s="100" t="n"/>
-      <c r="G26" s="101" t="n"/>
-      <c r="H26" s="100" t="n"/>
+      <c r="D26" s="102" t="n"/>
+      <c r="E26" s="99" t="n"/>
+      <c r="F26" s="101" t="n"/>
+      <c r="G26" s="102" t="n"/>
+      <c r="H26" s="101" t="n"/>
     </row>
     <row r="27" hidden="1" ht="26.25" customHeight="1">
       <c r="A27" s="10" t="n">
@@ -1388,11 +1459,11 @@
       </c>
       <c r="B27" s="14" t="n"/>
       <c r="C27" s="13" t="n"/>
-      <c r="D27" s="101" t="n"/>
-      <c r="E27" s="98" t="n"/>
-      <c r="F27" s="100" t="n"/>
-      <c r="G27" s="101" t="n"/>
-      <c r="H27" s="100" t="n"/>
+      <c r="D27" s="102" t="n"/>
+      <c r="E27" s="99" t="n"/>
+      <c r="F27" s="101" t="n"/>
+      <c r="G27" s="102" t="n"/>
+      <c r="H27" s="101" t="n"/>
     </row>
     <row r="28" hidden="1" ht="26.25" customHeight="1">
       <c r="A28" s="10" t="n">
@@ -1400,9 +1471,9 @@
       </c>
       <c r="B28" s="14" t="n"/>
       <c r="C28" s="13" t="n"/>
-      <c r="D28" s="101" t="n"/>
-      <c r="E28" s="98" t="n"/>
-      <c r="F28" s="100" t="n"/>
+      <c r="D28" s="102" t="n"/>
+      <c r="E28" s="99" t="n"/>
+      <c r="F28" s="101" t="n"/>
       <c r="G28" s="12" t="n"/>
       <c r="H28" s="11" t="n"/>
     </row>
@@ -1412,11 +1483,11 @@
       </c>
       <c r="B29" s="9" t="n"/>
       <c r="C29" s="8" t="n"/>
-      <c r="D29" s="102" t="n"/>
-      <c r="E29" s="98" t="n"/>
-      <c r="F29" s="100" t="n"/>
-      <c r="G29" s="101" t="n"/>
-      <c r="H29" s="100" t="n"/>
+      <c r="D29" s="103" t="n"/>
+      <c r="E29" s="99" t="n"/>
+      <c r="F29" s="101" t="n"/>
+      <c r="G29" s="102" t="n"/>
+      <c r="H29" s="101" t="n"/>
     </row>
     <row r="30" ht="30.75" customHeight="1">
       <c r="A30" s="86" t="inlineStr">
@@ -1424,7 +1495,11 @@
           <t>Observaciones:</t>
         </is>
       </c>
-      <c r="B30" s="103" t="inlineStr"/>
+      <c r="B30" s="104" t="inlineStr">
+        <is>
+          <t>Transferencia Electrónica</t>
+        </is>
+      </c>
       <c r="C30" s="90" t="n"/>
       <c r="D30" s="90" t="n"/>
       <c r="E30" s="90" t="n"/>
@@ -1438,7 +1513,11 @@
           <t>Proveedor:</t>
         </is>
       </c>
-      <c r="B31" s="104" t="inlineStr"/>
+      <c r="B31" s="105" t="inlineStr">
+        <is>
+          <t>9 - MANUEL NIETO HERNANDEZ</t>
+        </is>
+      </c>
       <c r="H31" s="92" t="n"/>
     </row>
     <row r="32">
@@ -1447,7 +1526,11 @@
           <t>Monto:</t>
         </is>
       </c>
-      <c r="B32" s="105" t="inlineStr"/>
+      <c r="B32" s="106" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
       <c r="C32" s="94" t="n"/>
       <c r="D32" s="94" t="n"/>
       <c r="E32" s="94" t="n"/>
@@ -1508,7 +1591,11 @@
           <t xml:space="preserve">Nombre: </t>
         </is>
       </c>
-      <c r="B39" s="106" t="inlineStr"/>
+      <c r="B39" s="107" t="inlineStr">
+        <is>
+          <t>Mishell Paola Sandoval Ramirez</t>
+        </is>
+      </c>
       <c r="C39" s="90" t="n"/>
       <c r="D39" s="1" t="n"/>
       <c r="G39" s="65" t="inlineStr">
@@ -1524,7 +1611,11 @@
           <t>Puesto:</t>
         </is>
       </c>
-      <c r="B40" s="78" t="inlineStr"/>
+      <c r="B40" s="78" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
       <c r="D40" s="1" t="n"/>
       <c r="G40" s="78" t="inlineStr">
         <is>

</xml_diff>